<commit_message>
updated version - updated tests
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -194,13 +248,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2">
@@ -208,7 +262,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -219,7 +273,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -230,7 +284,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
moved process testing into tmp
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -248,13 +266,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2">
@@ -262,7 +280,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -273,7 +291,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -284,7 +302,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
updated mcp and fixed documentation stdev
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -266,13 +284,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
@@ -280,7 +298,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -291,7 +309,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -302,7 +320,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
fixed runtime join issue with empty dataframes
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -320,13 +356,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2">
@@ -334,7 +370,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -345,7 +381,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -356,7 +392,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
updated createDataFrame to not accept generic type (was only used in specific test cases, no functionality change)
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -356,13 +374,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2">
@@ -370,7 +388,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -381,7 +399,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -392,7 +410,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
fix to summarize and slice with empty dataframes not preserving runtime columns
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -374,13 +392,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2">
@@ -388,7 +406,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -399,7 +417,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -410,7 +428,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
fix to summarize again - needed summary columns included not just group by vars
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -392,13 +428,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
@@ -406,7 +442,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -417,7 +453,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -428,7 +464,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
lint and fmt updates
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="138">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
   <si>
     <t>id</t>
   </si>
@@ -446,13 +464,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="C1" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2">
@@ -460,7 +478,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -471,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -482,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
improved speed of create dataframe by col
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie</t>
+  </si>
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -518,13 +572,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>150</v>
+        <v>168</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2">
@@ -532,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>153</v>
+        <v>171</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -543,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>172</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -554,7 +608,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>

<commit_message>
refactor(rename): implement via mutate+drop composition with improved types
- Rewrote rename.verb.ts to use mutate() + drop() instead of direct column manipulation
- Enhanced rename.types.ts with proper type inference via MutateAssignmentsFromRename
- Fixed mapping direction: now correctly maps oldKey -> newKey (was newKey -> oldKey)
- Added comprehensive type tests in rename.types.test.ts
- Simplified implementation from ~180 lines to ~70 lines
- Improved type safety with ProvidedKeys and NewKeyValues helpers
- Updated documentation and examples to reflect correct mapping direction
- Updated tests to use correct oldKey -> newKey syntax

This approach provides better type inference, eliminates view-specific logic, and
ensures consistency with other DataFrame operations by composing existing verbs.
</commit_message>
<xml_diff>
--- a/examples/fixtures/test-output.xlsx
+++ b/examples/fixtures/test-output.xlsx
@@ -8,7 +8,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bob</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charlie</t>
+  </si>
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -572,13 +608,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2">
@@ -586,7 +622,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="C2">
         <v>85</v>
@@ -597,7 +633,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="C3">
         <v>92</v>
@@ -608,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>173</v>
+        <v>185</v>
       </c>
       <c r="C4">
         <v>78</v>

</xml_diff>